<commit_message>
Package overhaul and new experiments and analyses
</commit_message>
<xml_diff>
--- a/metadata/30_GSE101968.xlsx
+++ b/metadata/30_GSE101968.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/krivi/Dropbox/Arbejde/kvs/projects/paired_gsea/01_currated_datasets/05_1_individual_study_excel_KVS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/sohdam_dtu_dk/Documents/Rprojects/pairedGSEA/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4DD1DE0-0E87-AA4C-8C1E-367181A91340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{D4DD1DE0-0E87-AA4C-8C1E-367181A91340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01DDC76F-DE2B-214D-B56C-2B6711E48DAB}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="37480" windowHeight="21140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20" yWindow="500" windowWidth="37480" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
     <t>1v2</t>
   </si>
   <si>
-    <t>Obstructed defecation symdrome</t>
+    <t>Obstructed defecation syndrome</t>
   </si>
 </sst>
 </file>
@@ -139,7 +139,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>

</xml_diff>